<commit_message>
Reorder backbone groups chart to same order as other
</commit_message>
<xml_diff>
--- a/charts.xlsx
+++ b/charts.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2740" yWindow="0" windowWidth="33360" windowHeight="22780" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="2740" yWindow="0" windowWidth="33360" windowHeight="22780" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="backbone" sheetId="1" r:id="rId1"/>
@@ -642,70 +642,76 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>backbone!$A$6:$A$26</c:f>
+              <c:f>backbone!$A$4:$A$26</c:f>
               <c:strCache>
-                <c:ptCount val="21"/>
+                <c:ptCount val="23"/>
                 <c:pt idx="0">
+                  <c:v>Chordata</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Mollusca</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>Arachnida</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="3">
                   <c:v>Curculionidae</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="4">
                   <c:v>Other Coleoptera</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="5">
                   <c:v>Diptera</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="6">
                   <c:v>Hemiptera</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="7">
                   <c:v>Hymenoptera</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="8">
                   <c:v>Lepidoptera</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="9">
                   <c:v>Other Insecta</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="10">
                   <c:v>Other Arthropoda</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="11">
                   <c:v>Other Animalia</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="12">
                   <c:v>Archaea</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="13">
                   <c:v>Bacteria</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="14">
                   <c:v>Chromista</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="15">
                   <c:v>Ascomycota</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="16">
                   <c:v>Other Fungi</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="17">
                   <c:v>Liliopsida</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="18">
                   <c:v>Magnoliopsida</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="19">
                   <c:v>Other Tracheophyta</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="20">
                   <c:v>Other Plantae</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="21">
                   <c:v>Protozoa</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="22">
                   <c:v>Viruses</c:v>
                 </c:pt>
               </c:strCache>
@@ -843,7 +849,7 @@
               <c:idx val="20"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-7.14973847711637E-17"/>
+                  <c:x val="-7.14973847711638E-17"/>
                   <c:y val="-0.00622406639004149"/>
                 </c:manualLayout>
               </c:layout>
@@ -894,70 +900,76 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>backbone!$A$6:$A$26</c:f>
+              <c:f>backbone!$A$4:$A$26</c:f>
               <c:strCache>
-                <c:ptCount val="21"/>
+                <c:ptCount val="23"/>
                 <c:pt idx="0">
+                  <c:v>Chordata</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Mollusca</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>Arachnida</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="3">
                   <c:v>Curculionidae</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="4">
                   <c:v>Other Coleoptera</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="5">
                   <c:v>Diptera</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="6">
                   <c:v>Hemiptera</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="7">
                   <c:v>Hymenoptera</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="8">
                   <c:v>Lepidoptera</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="9">
                   <c:v>Other Insecta</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="10">
                   <c:v>Other Arthropoda</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="11">
                   <c:v>Other Animalia</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="12">
                   <c:v>Archaea</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="13">
                   <c:v>Bacteria</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="14">
                   <c:v>Chromista</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="15">
                   <c:v>Ascomycota</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="16">
                   <c:v>Other Fungi</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="17">
                   <c:v>Liliopsida</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="18">
                   <c:v>Magnoliopsida</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="19">
                   <c:v>Other Tracheophyta</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="20">
                   <c:v>Other Plantae</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="21">
                   <c:v>Protozoa</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="22">
                   <c:v>Viruses</c:v>
                 </c:pt>
               </c:strCache>
@@ -965,71 +977,77 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>backbone!$C$6:$C$26</c:f>
+              <c:f>backbone!$C$4:$C$26</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="21"/>
+                <c:ptCount val="23"/>
                 <c:pt idx="0">
+                  <c:v>0.037199669184888</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0371822228831509</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>0.0439189876824956</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="3">
                   <c:v>0.0302178253849506</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="4">
                   <c:v>0.0904391358763672</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="5">
                   <c:v>0.0682520093362637</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="6">
                   <c:v>0.0334765453165611</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="7">
                   <c:v>0.0499392079462089</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="8">
                   <c:v>0.106789228320997</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="9">
                   <c:v>0.0383889254199678</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="10">
                   <c:v>0.0503890732981444</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="11">
                   <c:v>0.0537429171130358</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="12">
                   <c:v>0.000200217081840186</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="13">
                   <c:v>0.00757584883527243</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="14">
                   <c:v>0.025541801131268</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="15">
                   <c:v>0.057573211120605</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="16">
                   <c:v>0.0295083424476414</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="17">
                   <c:v>0.039569458504179</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="18">
                   <c:v>0.156086661596162</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="19">
                   <c:v>0.00935786394127741</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="20">
                   <c:v>0.0265208709692293</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="21">
                   <c:v>0.00547149253526749</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="22">
                   <c:v>0.00265848407422654</c:v>
                 </c:pt>
               </c:numCache>
@@ -1481,7 +1499,7 @@
               <c:idx val="20"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-7.14973847711639E-17"/>
+                  <c:x val="-7.1497384771164E-17"/>
                   <c:y val="-0.00622406639004149"/>
                 </c:manualLayout>
               </c:layout>
@@ -2105,8 +2123,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2505,7 +2523,6 @@
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.75000000000000011" right="0.75000000000000011" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Calibri,Regular"&amp;K000000GBIF Backbone Major Groups</oddHeader>
     <oddFooter>&amp;R&amp;"Calibri,Regular"&amp;K000000by number of species</oddFooter>
@@ -2523,7 +2540,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D1" sqref="D1:E1"/>
     </sheetView>
   </sheetViews>
@@ -3437,7 +3454,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>

<commit_message>
Add backbone august 2016 figures
</commit_message>
<xml_diff>
--- a/charts.xlsx
+++ b/charts.xlsx
@@ -11,7 +11,7 @@
     <sheet name="occurrences" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="occ_groups" localSheetId="1">occurrences!$A$3:$G$25</definedName>
+    <definedName name="occ_groups" localSheetId="1">occurrences!$A$3:$G$26</definedName>
   </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -36,11 +36,23 @@
       </textFields>
     </textPr>
   </connection>
+  <connection id="2" name="query_result.csv" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" sourceFile="Macintosh HD:Users:markus:Downloads:query_result.csv" decimal="," thousands="." comma="1">
+      <textFields count="6">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="58">
   <si>
     <t>name</t>
   </si>
@@ -114,9 +126,6 @@
     <t>Other Plantae</t>
   </si>
   <si>
-    <t>Curculionidae</t>
-  </si>
-  <si>
     <t>Mollusca</t>
   </si>
   <si>
@@ -129,9 +138,6 @@
     <t>Other Tracheophyta</t>
   </si>
   <si>
-    <t>Other Coleoptera</t>
-  </si>
-  <si>
     <t>rank</t>
   </si>
   <si>
@@ -202,13 +208,31 @@
   </si>
   <si>
     <t>3% cutoff</t>
+  </si>
+  <si>
+    <t>BACKBONE AUGUST 2016</t>
+  </si>
+  <si>
+    <t>Asterales</t>
+  </si>
+  <si>
+    <t>family</t>
+  </si>
+  <si>
+    <t>Asteraceae</t>
+  </si>
+  <si>
+    <t>Magnoliopsida other</t>
+  </si>
+  <si>
+    <t>Asterales other</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -264,29 +288,49 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
+      <i/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
+      <sz val="20"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="9"/>
-      <color theme="1"/>
+      <color theme="0" tint="-0.34998626667073579"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="0" tint="-0.34998626667073579"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
       <i/>
       <sz val="9"/>
-      <color theme="1"/>
+      <color theme="0" tint="-0.34998626667073579"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="12"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FFA6A6A6"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
@@ -317,7 +361,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="53">
+  <cellStyleXfs count="103">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -371,8 +415,58 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -381,15 +475,21 @@
     <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="3" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="3" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="53">
+  <cellStyles count="103">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -416,6 +516,31 @@
     <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -442,6 +567,31 @@
     <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -646,9 +796,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>backbone!$A$4:$A$26</c:f>
+              <c:f>backbone!$A$4:$A$25</c:f>
               <c:strCache>
-                <c:ptCount val="23"/>
+                <c:ptCount val="22"/>
                 <c:pt idx="0">
                   <c:v>Chordata</c:v>
                 </c:pt>
@@ -659,63 +809,60 @@
                   <c:v>Arachnida</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Curculionidae</c:v>
+                  <c:v>Coleoptera</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Other Coleoptera</c:v>
+                  <c:v>Diptera</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Diptera</c:v>
+                  <c:v>Hemiptera</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>Hemiptera</c:v>
+                  <c:v>Hymenoptera</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>Hymenoptera</c:v>
+                  <c:v>Lepidoptera</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>Lepidoptera</c:v>
+                  <c:v>Other Insecta</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>Other Insecta</c:v>
+                  <c:v>Other Arthropoda</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>Other Arthropoda</c:v>
+                  <c:v>Other Animalia</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>Other Animalia</c:v>
+                  <c:v>Archaea</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>Archaea</c:v>
+                  <c:v>Bacteria</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>Bacteria</c:v>
+                  <c:v>Chromista</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>Chromista</c:v>
+                  <c:v>Ascomycota</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>Ascomycota</c:v>
+                  <c:v>Other Fungi</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>Other Fungi</c:v>
+                  <c:v>Liliopsida</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>Liliopsida</c:v>
+                  <c:v>Magnoliopsida</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>Magnoliopsida</c:v>
+                  <c:v>Other Tracheophyta</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>Other Tracheophyta</c:v>
+                  <c:v>Other Plantae</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>Other Plantae</c:v>
+                  <c:v>Protozoa</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>Protozoa</c:v>
-                </c:pt>
-                <c:pt idx="22">
                   <c:v>Viruses</c:v>
                 </c:pt>
               </c:strCache>
@@ -728,28 +875,28 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>1.540573E6</c:v>
+                  <c:v>1.625418E6</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>482.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>18238.0</c:v>
+                  <c:v>18209.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>61489.0</c:v>
+                  <c:v>65321.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>209639.0</c:v>
+                  <c:v>209647.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>557394.0</c:v>
+                  <c:v>575225.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>13172.0</c:v>
+                  <c:v>13199.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6400.0</c:v>
+                  <c:v>6398.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -790,11 +937,15 @@
               <c:showBubbleSize val="0"/>
             </c:dLbl>
             <c:dLbl>
+              <c:idx val="11"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
               <c:idx val="12"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.00194995120131964"/>
-                  <c:y val="0.00726141078838174"/>
+                  <c:x val="-0.00194997613332638"/>
+                  <c:y val="0.00834870567152597"/>
                 </c:manualLayout>
               </c:layout>
               <c:showLegendKey val="0"/>
@@ -823,8 +974,8 @@
               <c:idx val="17"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.00899887514060742"/>
-                  <c:y val="-0.0217917675544794"/>
+                  <c:x val="0.015579991134572"/>
+                  <c:y val="-0.0207044784379039"/>
                 </c:manualLayout>
               </c:layout>
               <c:showLegendKey val="0"/>
@@ -838,10 +989,61 @@
               <c:idx val="18"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="0.00899887514060742"/>
-                  <c:y val="-0.0338983050847458"/>
+                  <c:x val="-0.00673159413432563"/>
+                  <c:y val="-0.0284619480159132"/>
                 </c:manualLayout>
               </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>Other </a:t>
+                    </a:r>
+                  </a:p>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>Tracheophyta, 1%</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="19"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.00196631044449918"/>
+                  <c:y val="0.0119599031317962"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>Other</a:t>
+                    </a:r>
+                  </a:p>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>Plantae, 2%</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
               <c:showCatName val="1"/>
@@ -853,8 +1055,8 @@
               <c:idx val="20"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-7.14973847711639E-17"/>
-                  <c:y val="-0.00622406639004149"/>
+                  <c:x val="0.00294946566674878"/>
+                  <c:y val="-0.0290568654230733"/>
                 </c:manualLayout>
               </c:layout>
               <c:showLegendKey val="0"/>
@@ -866,18 +1068,7 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="21"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="0.0"/>
-                  <c:y val="-0.0259336099585062"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="1"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
+              <c:delete val="1"/>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="22"/>
@@ -904,9 +1095,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>backbone!$A$4:$A$26</c:f>
+              <c:f>backbone!$A$4:$A$25</c:f>
               <c:strCache>
-                <c:ptCount val="23"/>
+                <c:ptCount val="22"/>
                 <c:pt idx="0">
                   <c:v>Chordata</c:v>
                 </c:pt>
@@ -917,63 +1108,60 @@
                   <c:v>Arachnida</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Curculionidae</c:v>
+                  <c:v>Coleoptera</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Other Coleoptera</c:v>
+                  <c:v>Diptera</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Diptera</c:v>
+                  <c:v>Hemiptera</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>Hemiptera</c:v>
+                  <c:v>Hymenoptera</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>Hymenoptera</c:v>
+                  <c:v>Lepidoptera</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>Lepidoptera</c:v>
+                  <c:v>Other Insecta</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>Other Insecta</c:v>
+                  <c:v>Other Arthropoda</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>Other Arthropoda</c:v>
+                  <c:v>Other Animalia</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>Other Animalia</c:v>
+                  <c:v>Archaea</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>Archaea</c:v>
+                  <c:v>Bacteria</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>Bacteria</c:v>
+                  <c:v>Chromista</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>Chromista</c:v>
+                  <c:v>Ascomycota</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>Ascomycota</c:v>
+                  <c:v>Other Fungi</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>Other Fungi</c:v>
+                  <c:v>Liliopsida</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>Liliopsida</c:v>
+                  <c:v>Magnoliopsida</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>Magnoliopsida</c:v>
+                  <c:v>Other Tracheophyta</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>Other Tracheophyta</c:v>
+                  <c:v>Other Plantae</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>Other Plantae</c:v>
+                  <c:v>Protozoa</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>Protozoa</c:v>
-                </c:pt>
-                <c:pt idx="22">
                   <c:v>Viruses</c:v>
                 </c:pt>
               </c:strCache>
@@ -981,78 +1169,75 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>backbone!$C$4:$C$26</c:f>
+              <c:f>backbone!$C$4:$C$25</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="23"/>
+                <c:ptCount val="22"/>
                 <c:pt idx="0">
-                  <c:v>0.037199669184888</c:v>
+                  <c:v>0.0401810096587015</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0371822228831509</c:v>
+                  <c:v>0.0424989229877573</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.0439189876824956</c:v>
+                  <c:v>0.0432439807645414</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.0302178253849506</c:v>
+                  <c:v>0.116746138170229</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.0904391358763672</c:v>
+                  <c:v>0.0678121913410204</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.0682520093362637</c:v>
+                  <c:v>0.0337141627408261</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.0334765453165611</c:v>
+                  <c:v>0.0493225861500402</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.0499392079462089</c:v>
+                  <c:v>0.102715741563205</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.106789228320997</c:v>
+                  <c:v>0.0397299175503869</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.0383889254199678</c:v>
+                  <c:v>0.0516568088057635</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.0503890732981444</c:v>
+                  <c:v>0.0589510557106709</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.0537429171130358</c:v>
+                  <c:v>0.000191734035456476</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.000200217081840186</c:v>
+                  <c:v>0.00724332998262858</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.00757584883527243</c:v>
+                  <c:v>0.0259839396889056</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.025541801131268</c:v>
+                  <c:v>0.0555965056670932</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.057573211120605</c:v>
+                  <c:v>0.0277986506220019</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.0295083424476414</c:v>
+                  <c:v>0.0398405027409613</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.039569458504179</c:v>
+                  <c:v>0.154878537284115</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.156086661596162</c:v>
+                  <c:v>0.00949163033200618</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.00935786394127741</c:v>
+                  <c:v>0.0246071938450988</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.0265208709692293</c:v>
+                  <c:v>0.00525040982155608</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.00547149253526749</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>0.00265848407422654</c:v>
+                  <c:v>0.0025450505370343</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1280,9 +1465,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>occurrences!$B$4:$B$25</c:f>
+              <c:f>occurrences!$B$4:$B$26</c:f>
               <c:strCache>
-                <c:ptCount val="22"/>
+                <c:ptCount val="23"/>
                 <c:pt idx="0">
                   <c:v>Chordata</c:v>
                 </c:pt>
@@ -1335,18 +1520,21 @@
                   <c:v>Liliopsida</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>Magnoliopsida</c:v>
+                  <c:v>Asteraceae</c:v>
                 </c:pt>
                 <c:pt idx="18">
+                  <c:v>Magnoliopsida other</c:v>
+                </c:pt>
+                <c:pt idx="19">
                   <c:v>Tracheophyta other</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="20">
                   <c:v>Plantae other</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="21">
                   <c:v>Protozoa</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="22">
                   <c:v>Viruses</c:v>
                 </c:pt>
               </c:strCache>
@@ -1354,33 +1542,33 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>occurrences!$E$30:$E$37</c:f>
+              <c:f>occurrences!$E$31:$E$38</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>681190.0</c:v>
+                  <c:v>698121.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>368.0</c:v>
+                  <c:v>372.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>12058.0</c:v>
+                  <c:v>12099.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>28898.0</c:v>
+                  <c:v>30611.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>104261.0</c:v>
+                  <c:v>102462.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>395897.0</c:v>
+                  <c:v>410464.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3152.0</c:v>
+                  <c:v>3262.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>63.0</c:v>
+                  <c:v>255.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1458,8 +1646,8 @@
               <c:idx val="17"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.00899887514060742"/>
-                  <c:y val="-0.0217917675544794"/>
+                  <c:x val="-0.00392798390059255"/>
+                  <c:y val="-0.00237426632350568"/>
                 </c:manualLayout>
               </c:layout>
               <c:showLegendKey val="0"/>
@@ -1473,10 +1661,28 @@
               <c:idx val="18"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.00824248135311686"/>
-                  <c:y val="-0.0338983284984114"/>
+                  <c:x val="-0.000128891089425181"/>
+                  <c:y val="-0.00908722574726703"/>
                 </c:manualLayout>
               </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>Magnoliopsida </a:t>
+                    </a:r>
+                  </a:p>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>other, 19%</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
               <c:showCatName val="1"/>
@@ -1492,6 +1698,24 @@
                   <c:y val="0.0131578947368421"/>
                 </c:manualLayout>
               </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>Tracheophyta </a:t>
+                    </a:r>
+                  </a:p>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>other, 1%</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
               <c:showCatName val="1"/>
@@ -1554,9 +1778,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>occurrences!$B$4:$B$25</c:f>
+              <c:f>occurrences!$B$4:$B$26</c:f>
               <c:strCache>
-                <c:ptCount val="22"/>
+                <c:ptCount val="23"/>
                 <c:pt idx="0">
                   <c:v>Chordata</c:v>
                 </c:pt>
@@ -1609,18 +1833,21 @@
                   <c:v>Liliopsida</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>Magnoliopsida</c:v>
+                  <c:v>Asteraceae</c:v>
                 </c:pt>
                 <c:pt idx="18">
+                  <c:v>Magnoliopsida other</c:v>
+                </c:pt>
+                <c:pt idx="19">
                   <c:v>Tracheophyta other</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="20">
                   <c:v>Plantae other</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="21">
                   <c:v>Protozoa</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="22">
                   <c:v>Viruses</c:v>
                 </c:pt>
               </c:strCache>
@@ -1628,75 +1855,78 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>occurrences!$F$4:$F$25</c:f>
+              <c:f>occurrences!$F$4:$F$26</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="22"/>
+                <c:ptCount val="23"/>
                 <c:pt idx="0">
-                  <c:v>0.0634047020647091</c:v>
+                  <c:v>0.0644084265365611</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0390133837784396</c:v>
+                  <c:v>0.0386444198128885</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.0164028168991106</c:v>
+                  <c:v>0.0196629258153725</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.0312328950384497</c:v>
+                  <c:v>0.0307177059363287</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.0800024798370486</c:v>
+                  <c:v>0.077135378317905</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.05258559720431</c:v>
+                  <c:v>0.0514397533169111</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.0481798077636846</c:v>
+                  <c:v>0.0473829678621806</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.0529844920453516</c:v>
+                  <c:v>0.0498168801077569</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.0579156153870626</c:v>
+                  <c:v>0.0576871393062913</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.0533899127733633</c:v>
+                  <c:v>0.0537170237093745</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.0605594153457863</c:v>
+                  <c:v>0.0644887353038931</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.000300190800620285</c:v>
+                  <c:v>0.00029579070740097</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.00983614313554185</c:v>
+                  <c:v>0.00962035421732347</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.0235731352074049</c:v>
+                  <c:v>0.0243399175920728</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.0569187861523941</c:v>
+                  <c:v>0.0548938254484966</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.028130651520083</c:v>
+                  <c:v>0.0265774311690253</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.0575183520177635</c:v>
+                  <c:v>0.0586659521041692</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.218706944441046</c:v>
+                  <c:v>0.029645067053845</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.0136211575781455</c:v>
+                  <c:v>0.194223970815317</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.033100930183614</c:v>
+                  <c:v>0.0136707785815722</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.00257119946618245</c:v>
+                  <c:v>0.0301690618822785</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>5.13913598887989E-5</c:v>
+                  <c:v>0.00259373464393001</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.000202759759105503</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1739,7 +1969,7 @@
     <xdr:to>
       <xdr:col>24</xdr:col>
       <xdr:colOff>338667</xdr:colOff>
-      <xdr:row>62</xdr:row>
+      <xdr:row>60</xdr:row>
       <xdr:rowOff>33867</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1774,7 +2004,7 @@
     <xdr:to>
       <xdr:col>25</xdr:col>
       <xdr:colOff>368301</xdr:colOff>
-      <xdr:row>61</xdr:row>
+      <xdr:row>62</xdr:row>
       <xdr:rowOff>25400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2125,10 +2355,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2140,18 +2370,22 @@
     <col min="7" max="7" width="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1">
+    <row r="1" spans="1:7" s="1" customFormat="1" ht="25">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="12">
+      <c r="B1" s="8">
         <f>SUM(F6:F13)</f>
-        <v>2407387</v>
+        <v>2513899</v>
       </c>
       <c r="C1" s="3">
         <f>B1*0.05</f>
-        <v>120369.35</v>
-      </c>
+        <v>125694.95000000001</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="F1" s="11"/>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="1" t="s">
@@ -2169,23 +2403,27 @@
         <v>21</v>
       </c>
       <c r="B4" s="4">
-        <v>89554</v>
+        <v>101011</v>
       </c>
       <c r="C4" s="6">
         <f>B4/$B$1</f>
-        <v>3.7199669184888012E-2</v>
+        <v>4.0181009658701486E-2</v>
+      </c>
+      <c r="D4">
+        <f>B4/$B$1</f>
+        <v>4.0181009658701486E-2</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B5" s="4">
-        <v>89512</v>
+        <v>106838</v>
       </c>
       <c r="C5" s="6">
-        <f>B5/$B$1</f>
-        <v>3.7182222883150901E-2</v>
+        <f t="shared" ref="C5:C25" si="0">B5/$B$1</f>
+        <v>4.2498922987757266E-2</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="17">
@@ -2193,33 +2431,33 @@
         <v>19</v>
       </c>
       <c r="B6" s="4">
-        <v>105730</v>
+        <v>108711</v>
       </c>
       <c r="C6" s="6">
-        <f t="shared" ref="C6:C26" si="0">B6/$B$1</f>
-        <v>4.3918987682495587E-2</v>
+        <f t="shared" si="0"/>
+        <v>4.3243980764541452E-2</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F6" s="5">
-        <v>1540573</v>
+        <v>1625418</v>
       </c>
       <c r="G6" s="6">
         <f t="shared" ref="G6:G13" si="1">F6/$B$1</f>
-        <v>0.63993574776303108</v>
+        <v>0.64657251544314231</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="17">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>46</v>
       </c>
       <c r="B7" s="4">
-        <v>72746</v>
+        <v>293488</v>
       </c>
       <c r="C7" s="6">
         <f t="shared" si="0"/>
-        <v>3.0217825384950572E-2</v>
+        <v>0.1167461381702288</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>5</v>
@@ -2229,117 +2467,117 @@
       </c>
       <c r="G7" s="6">
         <f t="shared" si="1"/>
-        <v>2.0021708184018606E-4</v>
+        <v>1.9173403545647618E-4</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="17">
       <c r="A8" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="B8" s="4">
-        <v>217722</v>
+        <v>170473</v>
       </c>
       <c r="C8" s="6">
         <f t="shared" si="0"/>
-        <v>9.0439135876367205E-2</v>
+        <v>6.7812191341020456E-2</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F8" s="5">
-        <v>18238</v>
+        <v>18209</v>
       </c>
       <c r="G8" s="6">
         <f t="shared" si="1"/>
-        <v>7.5758488352724342E-3</v>
+        <v>7.2433299826285781E-3</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="17">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="B9" s="4">
-        <v>164309</v>
+        <v>84754</v>
       </c>
       <c r="C9" s="6">
         <f t="shared" si="0"/>
-        <v>6.8252009336263755E-2</v>
+        <v>3.3714162740826101E-2</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>7</v>
       </c>
       <c r="F9" s="5">
-        <v>61489</v>
+        <v>65321</v>
       </c>
       <c r="G9" s="6">
         <f t="shared" si="1"/>
-        <v>2.5541801131268051E-2</v>
+        <v>2.5983939688905562E-2</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="17">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="B10" s="4">
-        <v>80591</v>
+        <v>123992</v>
       </c>
       <c r="C10" s="6">
         <f t="shared" si="0"/>
-        <v>3.3476545316561065E-2</v>
+        <v>4.9322586150040239E-2</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F10" s="5">
-        <v>209639</v>
+        <v>209647</v>
       </c>
       <c r="G10" s="6">
         <f t="shared" si="1"/>
-        <v>8.70815535682464E-2</v>
+        <v>8.3395156289095149E-2</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="17">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B11" s="4">
-        <v>120223</v>
+        <v>258217</v>
       </c>
       <c r="C11" s="6">
         <f t="shared" si="0"/>
-        <v>4.9939207946208895E-2</v>
+        <v>0.1027157415632052</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F11" s="5">
-        <v>557394</v>
+        <v>575225</v>
       </c>
       <c r="G11" s="6">
         <f t="shared" si="1"/>
-        <v>0.23153485501084786</v>
+        <v>0.22881786420218156</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="17">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="B12" s="4">
-        <v>257083</v>
+        <v>99877</v>
       </c>
       <c r="C12" s="6">
         <f t="shared" si="0"/>
-        <v>0.10678922832099699</v>
+        <v>3.9729917550386872E-2</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>4</v>
       </c>
       <c r="F12" s="5">
-        <v>13172</v>
+        <v>13199</v>
       </c>
       <c r="G12" s="6">
         <f t="shared" si="1"/>
-        <v>5.4714925352674915E-3</v>
+        <v>5.2504098215560768E-3</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="17">
@@ -2347,186 +2585,175 @@
         <v>26</v>
       </c>
       <c r="B13" s="4">
-        <v>92417</v>
+        <v>129860</v>
       </c>
       <c r="C13" s="6">
         <f t="shared" si="0"/>
-        <v>3.8388925419967794E-2</v>
+        <v>5.1656808805763475E-2</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F13" s="5">
-        <v>6400</v>
+        <v>6398</v>
       </c>
       <c r="G13" s="6">
         <f t="shared" si="1"/>
-        <v>2.6584840742265368E-3</v>
+        <v>2.5450505370343043E-3</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="B14" s="4">
-        <v>121306</v>
+        <v>148197</v>
       </c>
       <c r="C14" s="6">
         <f t="shared" si="0"/>
-        <v>5.0389073298144418E-2</v>
+        <v>5.8951055710670955E-2</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="B15" s="4">
-        <v>129380</v>
+        <v>482</v>
       </c>
       <c r="C15" s="6">
         <f t="shared" si="0"/>
-        <v>5.3742917113035832E-2</v>
+        <v>1.9173403545647618E-4</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B16" s="4">
-        <v>482</v>
+        <v>18209</v>
       </c>
       <c r="C16" s="6">
         <f t="shared" si="0"/>
-        <v>2.0021708184018606E-4</v>
+        <v>7.2433299826285781E-3</v>
       </c>
       <c r="E16" s="4">
-        <f>SUM(B6:B25)</f>
-        <v>2221921</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="17">
-      <c r="A17" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B17" s="5">
-        <v>18238</v>
+        <f>SUM(B4:B25)</f>
+        <v>2513899</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" s="4">
+        <v>65321</v>
       </c>
       <c r="C17" s="6">
         <f t="shared" si="0"/>
-        <v>7.5758488352724342E-3</v>
+        <v>2.5983939688905562E-2</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="B18" s="4">
-        <v>61489</v>
+        <v>139764</v>
       </c>
       <c r="C18" s="6">
         <f t="shared" si="0"/>
-        <v>2.5541801131268051E-2</v>
+        <v>5.5596505667093225E-2</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B19" s="4">
-        <v>138601</v>
+        <v>69883</v>
       </c>
       <c r="C19" s="6">
         <f t="shared" si="0"/>
-        <v>5.7573211120605039E-2</v>
+        <v>2.779865062200192E-2</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B20" s="4">
-        <v>71038</v>
+        <v>100155</v>
       </c>
       <c r="C20" s="6">
         <f t="shared" si="0"/>
-        <v>2.9508342447641365E-2</v>
+        <v>3.9840502740961355E-2</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B21" s="4">
-        <v>95259</v>
+        <v>389349</v>
       </c>
       <c r="C21" s="6">
         <f t="shared" si="0"/>
-        <v>3.9569458504179013E-2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="17">
-      <c r="A22" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B22" s="5">
-        <v>375761</v>
+        <v>0.15487853728411524</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" t="s">
+        <v>27</v>
+      </c>
+      <c r="B22" s="4">
+        <v>23861</v>
       </c>
       <c r="C22" s="6">
         <f t="shared" si="0"/>
-        <v>0.15608666159616214</v>
+        <v>9.4916303320061787E-3</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B23" s="4">
-        <v>22528</v>
+        <v>61860</v>
       </c>
       <c r="C23" s="6">
         <f t="shared" si="0"/>
-        <v>9.3578639412774094E-3</v>
+        <v>2.4607193845098789E-2</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="B24" s="4">
-        <v>63846</v>
+        <v>13199</v>
       </c>
       <c r="C24" s="6">
         <f t="shared" si="0"/>
-        <v>2.6520870969229293E-2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="A25" t="s">
-        <v>4</v>
-      </c>
-      <c r="B25" s="4">
-        <v>13172</v>
+        <v>5.2504098215560768E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="17">
+      <c r="A25" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B25" s="5">
+        <v>6398</v>
       </c>
       <c r="C25" s="6">
         <f t="shared" si="0"/>
-        <v>5.4714925352674915E-3</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="17">
-      <c r="A26" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B26" s="5">
-        <v>6400</v>
-      </c>
-      <c r="C26" s="6">
-        <f t="shared" si="0"/>
-        <v>2.6584840742265368E-3</v>
+        <v>2.5450505370343043E-3</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.75000000000000011" right="0.75000000000000011" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Calibri,Regular"&amp;K000000GBIF Backbone Major Groups</oddHeader>
     <oddFooter>&amp;R&amp;"Calibri,Regular"&amp;K000000by number of species</oddFooter>
@@ -2542,17 +2769,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J37"/>
+  <dimension ref="A1:J58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD6"/>
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="8.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11" customWidth="1"/>
@@ -2565,897 +2792,1066 @@
       <c r="A1" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="1">
-        <f>SUM(E30:E37)</f>
-        <v>1225887</v>
-      </c>
-      <c r="D1" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="E1" s="14">
+      <c r="B1" s="3">
+        <f>SUM(E31:E38)</f>
+        <v>1257646</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="E1" s="10">
         <f>B1*0.03</f>
-        <v>36776.61</v>
+        <v>37729.379999999997</v>
       </c>
     </row>
     <row r="3" spans="1:10" s="1" customFormat="1">
       <c r="A3" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="F3" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G3" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="H3" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="I3" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="G3" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="H3" s="9" t="s">
+      <c r="J3" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="I3" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B4" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="8">
+      <c r="C4" s="13">
         <v>44</v>
       </c>
-      <c r="D4" s="8">
+      <c r="D4" s="13">
         <v>1</v>
       </c>
       <c r="E4" s="4">
-        <v>77727</v>
+        <v>81003</v>
       </c>
       <c r="F4" s="6">
         <f t="shared" ref="F4:F14" si="0">E4/$B$1</f>
-        <v>6.3404702064709065E-2</v>
-      </c>
-      <c r="G4" s="10">
-        <v>166203</v>
-      </c>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10">
-        <v>77727</v>
+        <v>6.4408426536561161E-2</v>
+      </c>
+      <c r="G4" s="14">
+        <v>168031</v>
+      </c>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14">
+        <v>81003</v>
       </c>
       <c r="J4" s="4">
         <f>SUM(E4:E14)</f>
-        <v>681190</v>
+        <v>698121</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" t="s">
         <v>42</v>
       </c>
-      <c r="B5" t="s">
-        <v>44</v>
-      </c>
-      <c r="C5" s="8">
+      <c r="C5" s="13">
         <v>225</v>
       </c>
-      <c r="D5" s="8">
+      <c r="D5" s="13">
         <v>52</v>
       </c>
       <c r="E5" s="4">
-        <v>47826</v>
+        <v>48601</v>
       </c>
       <c r="F5" s="6">
         <f>E5/$B$1</f>
-        <v>3.901338377843961E-2</v>
-      </c>
-      <c r="G5" s="10">
-        <v>83454</v>
-      </c>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10">
-        <v>47826</v>
+        <v>3.8644419812888527E-2</v>
+      </c>
+      <c r="G5" s="14">
+        <v>83664</v>
+      </c>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14">
+        <v>48601</v>
       </c>
     </row>
     <row r="6" spans="1:10">
       <c r="B6" t="s">
-        <v>43</v>
-      </c>
-      <c r="C6" s="8">
+        <v>41</v>
+      </c>
+      <c r="C6" s="13">
         <v>52</v>
       </c>
-      <c r="D6" s="8">
+      <c r="D6" s="13">
         <v>1</v>
       </c>
       <c r="E6" s="4">
-        <v>20108</v>
+        <f t="shared" ref="E6" si="1">H6</f>
+        <v>24729</v>
       </c>
       <c r="F6" s="6">
         <f>E6/$B$1</f>
-        <v>1.6402816899110603E-2</v>
-      </c>
-      <c r="G6" s="10">
-        <v>125824</v>
-      </c>
-      <c r="H6" s="10">
+        <v>1.9662925815372528E-2</v>
+      </c>
+      <c r="G6" s="14">
+        <v>130281</v>
+      </c>
+      <c r="H6" s="14">
         <f>I6-I5</f>
-        <v>20108</v>
-      </c>
-      <c r="I6" s="11">
-        <v>67934</v>
+        <v>24729</v>
+      </c>
+      <c r="I6" s="15">
+        <v>73330</v>
       </c>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B7" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="8">
+      <c r="C7" s="13">
         <v>367</v>
       </c>
-      <c r="D7" s="8">
+      <c r="D7" s="13">
         <v>54</v>
       </c>
       <c r="E7" s="4">
-        <v>38288</v>
+        <v>38632</v>
       </c>
       <c r="F7" s="6">
         <f t="shared" si="0"/>
-        <v>3.1232895038449709E-2</v>
-      </c>
-      <c r="G7" s="10">
-        <v>48386</v>
-      </c>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10">
-        <v>38288</v>
+        <v>3.0717705936328665E-2</v>
+      </c>
+      <c r="G7" s="14">
+        <v>48440</v>
+      </c>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14">
+        <v>38632</v>
       </c>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B8" t="s">
-        <v>48</v>
-      </c>
-      <c r="C8" s="8">
+        <v>46</v>
+      </c>
+      <c r="C8" s="13">
         <v>1470</v>
       </c>
-      <c r="D8" s="8">
+      <c r="D8" s="13">
         <v>216</v>
       </c>
       <c r="E8" s="4">
-        <v>98074</v>
+        <v>97009</v>
       </c>
       <c r="F8" s="6">
         <f t="shared" si="0"/>
-        <v>8.0002479837048598E-2</v>
-      </c>
-      <c r="G8" s="10">
-        <v>128222</v>
-      </c>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10">
-        <v>98074</v>
+        <v>7.713537831790504E-2</v>
+      </c>
+      <c r="G8" s="14">
+        <v>126006</v>
+      </c>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14">
+        <v>97009</v>
       </c>
     </row>
     <row r="9" spans="1:10">
       <c r="A9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B9" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="8">
+      <c r="C9" s="13">
         <v>811</v>
       </c>
-      <c r="D9" s="8">
+      <c r="D9" s="13">
         <v>216</v>
       </c>
       <c r="E9" s="4">
-        <v>64464</v>
+        <v>64693</v>
       </c>
       <c r="F9" s="6">
         <f t="shared" si="0"/>
-        <v>5.2585597204310025E-2</v>
-      </c>
-      <c r="G9" s="10">
-        <v>75990</v>
-      </c>
-      <c r="H9" s="10"/>
-      <c r="I9" s="10">
-        <v>64464</v>
+        <v>5.143975331691112E-2</v>
+      </c>
+      <c r="G9" s="14">
+        <v>76047</v>
+      </c>
+      <c r="H9" s="14"/>
+      <c r="I9" s="14">
+        <v>64693</v>
       </c>
     </row>
     <row r="10" spans="1:10">
       <c r="A10" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B10" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="8">
+      <c r="C10" s="13">
         <v>1457</v>
       </c>
-      <c r="D10" s="8">
+      <c r="D10" s="13">
         <v>216</v>
       </c>
       <c r="E10" s="4">
-        <v>59063</v>
+        <v>59591</v>
       </c>
       <c r="F10" s="6">
         <f t="shared" si="0"/>
-        <v>4.8179807763684579E-2</v>
-      </c>
-      <c r="G10" s="10">
-        <v>75504</v>
-      </c>
-      <c r="H10" s="10"/>
-      <c r="I10" s="10">
-        <v>59063</v>
+        <v>4.7382967862180617E-2</v>
+      </c>
+      <c r="G10" s="14">
+        <v>75108</v>
+      </c>
+      <c r="H10" s="14"/>
+      <c r="I10" s="14">
+        <v>59591</v>
       </c>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B11" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="8">
+      <c r="C11" s="13">
         <v>797</v>
       </c>
-      <c r="D11" s="8">
+      <c r="D11" s="13">
         <v>216</v>
       </c>
       <c r="E11" s="4">
-        <v>64953</v>
+        <v>62652</v>
       </c>
       <c r="F11" s="6">
         <f t="shared" si="0"/>
-        <v>5.2984492045351654E-2</v>
-      </c>
-      <c r="G11" s="10">
-        <v>78547</v>
-      </c>
-      <c r="H11" s="10"/>
-      <c r="I11" s="10">
-        <v>64953</v>
+        <v>4.9816880107756874E-2</v>
+      </c>
+      <c r="G11" s="14">
+        <v>75400</v>
+      </c>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14">
+        <v>62652</v>
       </c>
     </row>
     <row r="12" spans="1:10">
       <c r="B12" t="s">
-        <v>46</v>
-      </c>
-      <c r="C12" s="8">
+        <v>44</v>
+      </c>
+      <c r="C12" s="13">
         <v>216</v>
       </c>
-      <c r="D12" s="8">
+      <c r="D12" s="13">
         <v>54</v>
       </c>
       <c r="E12" s="4">
-        <v>70998</v>
+        <f t="shared" ref="E12:E13" si="2">H12</f>
+        <v>72550</v>
       </c>
       <c r="F12" s="6">
         <f t="shared" si="0"/>
-        <v>5.7915615387062594E-2</v>
-      </c>
-      <c r="G12" s="10">
-        <v>449853</v>
-      </c>
-      <c r="H12" s="10">
+        <v>5.7687139306291275E-2</v>
+      </c>
+      <c r="G12" s="14">
+        <v>444929</v>
+      </c>
+      <c r="H12" s="14">
         <f>I12-SUM(I8:I11)</f>
-        <v>70998</v>
-      </c>
-      <c r="I12" s="11">
-        <v>357552</v>
+        <v>72550</v>
+      </c>
+      <c r="I12" s="15">
+        <v>356495</v>
       </c>
     </row>
     <row r="13" spans="1:10">
       <c r="B13" t="s">
-        <v>41</v>
-      </c>
-      <c r="C13" s="8">
+        <v>39</v>
+      </c>
+      <c r="C13" s="13">
         <v>54</v>
       </c>
-      <c r="D13" s="8">
+      <c r="D13" s="13">
         <v>1</v>
       </c>
       <c r="E13" s="4">
-        <v>65450</v>
+        <f t="shared" si="2"/>
+        <v>67557</v>
       </c>
       <c r="F13" s="6">
         <f t="shared" si="0"/>
-        <v>5.3389912773363288E-2</v>
-      </c>
-      <c r="G13" s="10">
-        <v>590978</v>
-      </c>
-      <c r="H13" s="10">
+        <v>5.3717023709374499E-2</v>
+      </c>
+      <c r="G13" s="14">
+        <v>588135</v>
+      </c>
+      <c r="H13" s="14">
         <f>I13-I7-I12</f>
-        <v>65450</v>
-      </c>
-      <c r="I13" s="10">
-        <v>461290</v>
+        <v>67557</v>
+      </c>
+      <c r="I13" s="14">
+        <v>462684</v>
       </c>
     </row>
     <row r="14" spans="1:10">
       <c r="B14" t="s">
-        <v>36</v>
-      </c>
-      <c r="C14" s="8">
+        <v>34</v>
+      </c>
+      <c r="C14" s="13">
         <v>1</v>
       </c>
-      <c r="D14" s="8"/>
+      <c r="D14" s="13"/>
       <c r="E14" s="4">
-        <v>74239</v>
+        <f>H14</f>
+        <v>81104</v>
       </c>
       <c r="F14" s="6">
         <f t="shared" si="0"/>
-        <v>6.0559415345786356E-2</v>
-      </c>
-      <c r="G14" s="10">
-        <v>1001540</v>
-      </c>
-      <c r="H14" s="10">
+        <v>6.4488735303893152E-2</v>
+      </c>
+      <c r="G14" s="14">
+        <v>1012631</v>
+      </c>
+      <c r="H14" s="14">
         <f>I14-I4-I13-I6</f>
-        <v>74239</v>
-      </c>
-      <c r="I14" s="10">
-        <v>681190</v>
+        <v>81104</v>
+      </c>
+      <c r="I14" s="14">
+        <v>698121</v>
       </c>
     </row>
     <row r="15" spans="1:10">
       <c r="A15" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B15" t="s">
         <v>5</v>
       </c>
-      <c r="C15" s="8">
+      <c r="C15" s="13">
         <v>2</v>
       </c>
-      <c r="D15" s="8"/>
+      <c r="D15" s="13"/>
       <c r="E15" s="4">
-        <v>368</v>
+        <v>372</v>
       </c>
       <c r="F15" s="6">
-        <f t="shared" ref="F15:F37" si="1">E15/$B$1</f>
-        <v>3.0019080062028555E-4</v>
-      </c>
-      <c r="G15" s="10">
-        <v>478</v>
-      </c>
-      <c r="H15" s="10"/>
-      <c r="I15" s="10">
-        <v>368</v>
+        <f t="shared" ref="F15:F19" si="3">E15/$B$1</f>
+        <v>2.9579070740096976E-4</v>
+      </c>
+      <c r="G15" s="14">
+        <v>481</v>
+      </c>
+      <c r="H15" s="14"/>
+      <c r="I15" s="14">
+        <v>372</v>
       </c>
       <c r="J15" s="4">
         <f>E15</f>
-        <v>368</v>
+        <v>372</v>
       </c>
     </row>
     <row r="16" spans="1:10">
       <c r="A16" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B16" t="s">
         <v>6</v>
       </c>
-      <c r="C16" s="8">
+      <c r="C16" s="13">
         <v>3</v>
       </c>
-      <c r="D16" s="8"/>
+      <c r="D16" s="13"/>
       <c r="E16" s="4">
-        <v>12058</v>
+        <v>12099</v>
       </c>
       <c r="F16" s="6">
-        <f t="shared" si="1"/>
-        <v>9.8361431355418558E-3</v>
-      </c>
-      <c r="G16" s="10">
-        <v>16801</v>
-      </c>
-      <c r="H16" s="10"/>
-      <c r="I16" s="10">
-        <v>12058</v>
+        <f t="shared" si="3"/>
+        <v>9.6203542173234763E-3</v>
+      </c>
+      <c r="G16" s="14">
+        <v>17094</v>
+      </c>
+      <c r="H16" s="14"/>
+      <c r="I16" s="14">
+        <v>12099</v>
       </c>
       <c r="J16" s="4">
-        <f t="shared" ref="J16:J17" si="2">E16</f>
-        <v>12058</v>
+        <f t="shared" ref="J16:J17" si="4">E16</f>
+        <v>12099</v>
       </c>
     </row>
     <row r="17" spans="1:10">
       <c r="A17" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B17" t="s">
         <v>7</v>
       </c>
-      <c r="C17" s="8">
+      <c r="C17" s="13">
         <v>4</v>
       </c>
-      <c r="D17" s="8"/>
+      <c r="D17" s="13"/>
       <c r="E17" s="4">
-        <v>28898</v>
+        <v>30611</v>
       </c>
       <c r="F17" s="6">
-        <f t="shared" si="1"/>
-        <v>2.3573135207404925E-2</v>
-      </c>
-      <c r="G17" s="10">
-        <v>41235</v>
-      </c>
-      <c r="H17" s="10"/>
-      <c r="I17" s="10">
-        <v>28898</v>
+        <f t="shared" si="3"/>
+        <v>2.433991759207281E-2</v>
+      </c>
+      <c r="G17" s="14">
+        <v>44152</v>
+      </c>
+      <c r="H17" s="14"/>
+      <c r="I17" s="14">
+        <v>30611</v>
       </c>
       <c r="J17" s="4">
-        <f t="shared" si="2"/>
-        <v>28898</v>
+        <f t="shared" si="4"/>
+        <v>30611</v>
       </c>
     </row>
     <row r="18" spans="1:10">
       <c r="A18" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B18" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="8">
+      <c r="C18" s="13">
         <v>95</v>
       </c>
-      <c r="D18" s="8">
+      <c r="D18" s="13">
         <v>5</v>
       </c>
       <c r="E18" s="4">
-        <v>69776</v>
+        <v>69037</v>
       </c>
       <c r="F18" s="6">
         <f>E18/$B$1</f>
-        <v>5.6918786152394145E-2</v>
-      </c>
-      <c r="G18" s="10">
-        <v>106025</v>
-      </c>
-      <c r="H18" s="10"/>
-      <c r="I18" s="10">
-        <v>69776</v>
+        <v>5.4893825448496636E-2</v>
+      </c>
+      <c r="G18" s="14">
+        <v>107426</v>
+      </c>
+      <c r="H18" s="14"/>
+      <c r="I18" s="14">
+        <v>69037</v>
       </c>
       <c r="J18" s="4">
         <f>E18+E19</f>
-        <v>104261</v>
+        <v>102462</v>
       </c>
     </row>
     <row r="19" spans="1:10">
       <c r="B19" t="s">
-        <v>38</v>
-      </c>
-      <c r="C19" s="8">
+        <v>36</v>
+      </c>
+      <c r="C19" s="13">
         <v>5</v>
       </c>
-      <c r="D19" s="8"/>
+      <c r="D19" s="13"/>
       <c r="E19" s="4">
-        <v>34485</v>
+        <f>H19</f>
+        <v>33425</v>
       </c>
       <c r="F19" s="6">
-        <f t="shared" si="1"/>
-        <v>2.8130651520083011E-2</v>
-      </c>
-      <c r="G19" s="10">
-        <v>158804</v>
-      </c>
-      <c r="H19" s="10">
+        <f t="shared" si="3"/>
+        <v>2.6577431169025306E-2</v>
+      </c>
+      <c r="G19" s="14">
+        <v>161732</v>
+      </c>
+      <c r="H19" s="14">
         <f>I19-I18</f>
-        <v>34485</v>
-      </c>
-      <c r="I19" s="10">
-        <v>104261</v>
+        <v>33425</v>
+      </c>
+      <c r="I19" s="14">
+        <v>102462</v>
       </c>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B20" t="s">
         <v>22</v>
       </c>
-      <c r="C20" s="8">
+      <c r="C20" s="13">
         <v>196</v>
       </c>
-      <c r="D20" s="8">
+      <c r="D20" s="13">
         <v>7707728</v>
       </c>
       <c r="E20" s="4">
-        <v>70511</v>
+        <v>73781</v>
       </c>
       <c r="F20" s="6">
         <f>E20/$B$1</f>
-        <v>5.7518352017763466E-2</v>
-      </c>
-      <c r="G20" s="10">
-        <v>151566</v>
-      </c>
-      <c r="H20" s="10"/>
-      <c r="I20" s="10">
-        <v>70511</v>
+        <v>5.8665952104169215E-2</v>
+      </c>
+      <c r="G20" s="14">
+        <v>162609</v>
+      </c>
+      <c r="H20" s="14"/>
+      <c r="I20" s="14">
+        <v>73781</v>
       </c>
       <c r="J20" s="4">
-        <f>SUM(E20:E23)</f>
-        <v>395897</v>
+        <f>SUM(E20:E24)</f>
+        <v>410464</v>
       </c>
     </row>
     <row r="21" spans="1:10">
-      <c r="A21" t="s">
-        <v>42</v>
-      </c>
-      <c r="B21" t="s">
-        <v>16</v>
-      </c>
-      <c r="C21" s="8">
+      <c r="A21" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="B21" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="C21" s="20">
+        <v>3065</v>
+      </c>
+      <c r="D21" s="20">
+        <v>414</v>
+      </c>
+      <c r="E21" s="16">
+        <v>37283</v>
+      </c>
+      <c r="F21" s="6">
+        <f t="shared" ref="F21:F28" si="5">E21/$B$1</f>
+        <v>2.964506705384504E-2</v>
+      </c>
+      <c r="G21" s="20">
+        <v>84190</v>
+      </c>
+      <c r="H21" s="17"/>
+      <c r="I21" s="20">
+        <v>37283</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="A22" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="B22" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="C22" s="18">
         <v>220</v>
       </c>
-      <c r="D21" s="8">
+      <c r="D22" s="18">
         <v>7707728</v>
       </c>
-      <c r="E21" s="4">
-        <v>268110</v>
-      </c>
-      <c r="F21" s="6">
-        <f>E21/$B$1</f>
-        <v>0.21870694444104555</v>
-      </c>
-      <c r="G21" s="10">
-        <v>571090</v>
-      </c>
-      <c r="H21" s="10"/>
-      <c r="I21" s="10">
-        <v>268110</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10">
-      <c r="B22" t="s">
-        <v>45</v>
-      </c>
-      <c r="C22" s="8">
-        <v>7707728</v>
-      </c>
-      <c r="D22" s="8">
-        <v>6</v>
-      </c>
-      <c r="E22" s="4">
-        <v>16698</v>
+      <c r="E22" s="16">
+        <f>H22</f>
+        <v>244265</v>
       </c>
       <c r="F22" s="6">
-        <f>E22/$B$1</f>
-        <v>1.3621157578145457E-2</v>
-      </c>
-      <c r="G22" s="10">
-        <v>761788</v>
-      </c>
-      <c r="H22" s="10">
-        <f>I22-I20-I21</f>
-        <v>16698</v>
-      </c>
-      <c r="I22" s="11">
-        <v>355319</v>
+        <f t="shared" si="5"/>
+        <v>0.19422397081531687</v>
+      </c>
+      <c r="G22" s="20">
+        <v>616429</v>
+      </c>
+      <c r="H22" s="20">
+        <f>I22-E21</f>
+        <v>244265</v>
+      </c>
+      <c r="I22" s="20">
+        <v>281548</v>
       </c>
     </row>
     <row r="23" spans="1:10">
       <c r="B23" t="s">
-        <v>39</v>
-      </c>
-      <c r="C23" s="8">
+        <v>43</v>
+      </c>
+      <c r="C23" s="13">
+        <v>7707728</v>
+      </c>
+      <c r="D23" s="13">
         <v>6</v>
       </c>
-      <c r="D23" s="8"/>
       <c r="E23" s="4">
-        <v>40578</v>
+        <f>H23</f>
+        <v>17193</v>
       </c>
       <c r="F23" s="6">
-        <f t="shared" si="1"/>
-        <v>3.3100930183613986E-2</v>
-      </c>
-      <c r="G23" s="10">
-        <v>833656</v>
-      </c>
-      <c r="H23" s="10">
-        <f>I23-I22</f>
-        <v>40578</v>
-      </c>
-      <c r="I23" s="10">
-        <v>395897</v>
+        <f t="shared" si="5"/>
+        <v>1.367077858157224E-2</v>
+      </c>
+      <c r="G23" s="14">
+        <v>822437</v>
+      </c>
+      <c r="H23" s="14">
+        <f>I23-E22-E21-E20</f>
+        <v>17193</v>
+      </c>
+      <c r="I23" s="15">
+        <v>372522</v>
       </c>
     </row>
     <row r="24" spans="1:10">
-      <c r="A24" t="s">
+      <c r="B24" t="s">
         <v>37</v>
       </c>
-      <c r="B24" t="s">
-        <v>4</v>
-      </c>
-      <c r="C24" s="8">
-        <v>7</v>
-      </c>
-      <c r="D24" s="8"/>
+      <c r="C24" s="13">
+        <v>6</v>
+      </c>
+      <c r="D24" s="13"/>
       <c r="E24" s="4">
-        <v>3152</v>
+        <f>H24</f>
+        <v>37942</v>
       </c>
       <c r="F24" s="6">
-        <f t="shared" si="1"/>
-        <v>2.5711994661824457E-3</v>
-      </c>
-      <c r="G24" s="10">
-        <v>6197</v>
-      </c>
-      <c r="H24" s="10"/>
-      <c r="I24" s="10">
-        <v>3152</v>
-      </c>
-      <c r="J24" s="4">
-        <f>E24</f>
-        <v>3152</v>
+        <f t="shared" si="5"/>
+        <v>3.016906188227848E-2</v>
+      </c>
+      <c r="G24" s="14">
+        <v>894184</v>
+      </c>
+      <c r="H24" s="14">
+        <f>I24-I23</f>
+        <v>37942</v>
+      </c>
+      <c r="I24" s="14">
+        <v>410464</v>
       </c>
     </row>
     <row r="25" spans="1:10">
       <c r="A25" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B25" t="s">
-        <v>3</v>
-      </c>
-      <c r="C25" s="8">
-        <v>8</v>
-      </c>
-      <c r="D25" s="8"/>
+        <v>4</v>
+      </c>
+      <c r="C25" s="13">
+        <v>7</v>
+      </c>
+      <c r="D25" s="13"/>
       <c r="E25" s="4">
-        <v>63</v>
+        <v>3262</v>
       </c>
       <c r="F25" s="6">
-        <f t="shared" si="1"/>
-        <v>5.1391359888798887E-5</v>
-      </c>
-      <c r="G25" s="10">
-        <v>89</v>
-      </c>
-      <c r="H25" s="10"/>
-      <c r="I25" s="10">
-        <v>63</v>
+        <f t="shared" si="5"/>
+        <v>2.593734643930009E-3</v>
+      </c>
+      <c r="G25" s="14">
+        <v>5357</v>
+      </c>
+      <c r="H25" s="14"/>
+      <c r="I25" s="14">
+        <v>3262</v>
       </c>
       <c r="J25" s="4">
         <f>E25</f>
-        <v>63</v>
+        <v>3262</v>
       </c>
     </row>
     <row r="26" spans="1:10">
-      <c r="E26" s="4"/>
-      <c r="F26" s="6"/>
-      <c r="G26" s="4"/>
-      <c r="H26" s="4"/>
-      <c r="I26" s="4"/>
+      <c r="A26" t="s">
+        <v>35</v>
+      </c>
+      <c r="B26" t="s">
+        <v>3</v>
+      </c>
+      <c r="C26" s="13">
+        <v>8</v>
+      </c>
+      <c r="D26" s="13"/>
+      <c r="E26" s="4">
+        <v>255</v>
+      </c>
+      <c r="F26" s="6">
+        <f t="shared" si="5"/>
+        <v>2.0275975910550345E-4</v>
+      </c>
+      <c r="G26" s="14">
+        <v>305</v>
+      </c>
+      <c r="H26" s="14"/>
+      <c r="I26" s="14">
+        <v>255</v>
+      </c>
+      <c r="J26" s="4">
+        <f>E26</f>
+        <v>255</v>
+      </c>
     </row>
     <row r="27" spans="1:10">
-      <c r="E27" s="4"/>
-      <c r="F27" s="6"/>
-      <c r="G27" s="4"/>
-      <c r="H27" s="4"/>
-      <c r="I27" s="4"/>
+      <c r="A27" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="B27" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="C27" s="20">
+        <v>3065</v>
+      </c>
+      <c r="D27" s="20">
+        <v>414</v>
+      </c>
+      <c r="E27" s="16">
+        <v>37283</v>
+      </c>
+      <c r="F27" s="6">
+        <f>E27/$B$1</f>
+        <v>2.964506705384504E-2</v>
+      </c>
+      <c r="G27" s="20">
+        <v>84190</v>
+      </c>
+      <c r="H27" s="17"/>
+      <c r="I27" s="20">
+        <v>37283</v>
+      </c>
     </row>
     <row r="28" spans="1:10">
-      <c r="E28" s="4"/>
-      <c r="F28" s="6"/>
-      <c r="G28" s="4"/>
-      <c r="H28" s="4"/>
-      <c r="I28" s="4"/>
-    </row>
-    <row r="29" spans="1:10" ht="20">
-      <c r="A29" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="E29" s="4"/>
-      <c r="F29" s="6"/>
-      <c r="G29" s="4"/>
-      <c r="H29" s="4"/>
-      <c r="I29" s="4"/>
-    </row>
-    <row r="30" spans="1:10">
-      <c r="A30" t="s">
-        <v>37</v>
-      </c>
-      <c r="B30" t="s">
-        <v>2</v>
-      </c>
-      <c r="C30">
-        <v>1</v>
-      </c>
-      <c r="E30" s="4">
-        <v>681190</v>
-      </c>
-      <c r="F30" s="6">
-        <f t="shared" si="1"/>
-        <v>0.55567111813731607</v>
-      </c>
-      <c r="G30" s="4">
-        <v>1001540</v>
-      </c>
+      <c r="A28" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="B28" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="C28" s="20">
+        <v>414</v>
+      </c>
+      <c r="D28" s="20">
+        <v>220</v>
+      </c>
+      <c r="E28" s="16">
+        <v>41066</v>
+      </c>
+      <c r="F28" s="6">
+        <f t="shared" si="5"/>
+        <v>3.265306771539845E-2</v>
+      </c>
+      <c r="G28" s="20">
+        <v>92377</v>
+      </c>
+      <c r="H28" s="17"/>
+      <c r="I28" s="20">
+        <v>41066</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" ht="20">
+      <c r="A30" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="E30" s="4"/>
+      <c r="F30" s="6"/>
+      <c r="G30" s="4"/>
       <c r="H30" s="4"/>
       <c r="I30" s="4"/>
     </row>
     <row r="31" spans="1:10">
       <c r="A31" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B31" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C31">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E31" s="4">
-        <v>368</v>
+        <v>698121</v>
       </c>
       <c r="F31" s="6">
-        <f t="shared" si="1"/>
-        <v>3.0019080062028555E-4</v>
+        <f>E31/$B$1</f>
+        <v>0.5551013560254634</v>
       </c>
       <c r="G31" s="4">
-        <v>478</v>
+        <v>1012631</v>
       </c>
       <c r="H31" s="4"/>
       <c r="I31" s="4"/>
     </row>
     <row r="32" spans="1:10">
       <c r="A32" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B32" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C32">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E32" s="4">
-        <v>12058</v>
+        <v>372</v>
       </c>
       <c r="F32" s="6">
-        <f t="shared" si="1"/>
-        <v>9.8361431355418558E-3</v>
+        <f>E32/$B$1</f>
+        <v>2.9579070740096976E-4</v>
       </c>
       <c r="G32" s="4">
-        <v>16801</v>
+        <v>481</v>
       </c>
       <c r="H32" s="4"/>
       <c r="I32" s="4"/>
     </row>
-    <row r="33" spans="1:9">
+    <row r="33" spans="1:10">
       <c r="A33" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B33" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C33">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E33" s="4">
-        <v>28898</v>
+        <v>12099</v>
       </c>
       <c r="F33" s="6">
-        <f t="shared" si="1"/>
-        <v>2.3573135207404925E-2</v>
+        <f>E33/$B$1</f>
+        <v>9.6203542173234763E-3</v>
       </c>
       <c r="G33" s="4">
-        <v>41235</v>
+        <v>17094</v>
       </c>
       <c r="H33" s="4"/>
       <c r="I33" s="4"/>
     </row>
-    <row r="34" spans="1:9">
+    <row r="34" spans="1:10">
       <c r="A34" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B34" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C34">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E34" s="4">
-        <v>104261</v>
+        <v>30611</v>
       </c>
       <c r="F34" s="6">
-        <f t="shared" si="1"/>
-        <v>8.5049437672477149E-2</v>
+        <f>E34/$B$1</f>
+        <v>2.433991759207281E-2</v>
       </c>
       <c r="G34" s="4">
-        <v>158804</v>
+        <v>44152</v>
       </c>
       <c r="H34" s="4"/>
       <c r="I34" s="4"/>
     </row>
-    <row r="35" spans="1:9">
+    <row r="35" spans="1:10">
       <c r="A35" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B35" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C35">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E35" s="4">
-        <v>395897</v>
+        <v>102462</v>
       </c>
       <c r="F35" s="6">
-        <f t="shared" si="1"/>
-        <v>0.32294738422056846</v>
+        <f>E35/$B$1</f>
+        <v>8.1471256617521942E-2</v>
       </c>
       <c r="G35" s="4">
-        <v>833656</v>
+        <v>161732</v>
       </c>
       <c r="H35" s="4"/>
       <c r="I35" s="4"/>
     </row>
-    <row r="36" spans="1:9">
+    <row r="36" spans="1:10">
       <c r="A36" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C36">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E36" s="4">
-        <v>3152</v>
+        <v>410464</v>
       </c>
       <c r="F36" s="6">
-        <f t="shared" si="1"/>
-        <v>2.5711994661824457E-3</v>
+        <f>E36/$B$1</f>
+        <v>0.32637483043718185</v>
       </c>
       <c r="G36" s="4">
-        <v>6197</v>
+        <v>894184</v>
       </c>
       <c r="H36" s="4"/>
       <c r="I36" s="4"/>
     </row>
-    <row r="37" spans="1:9">
+    <row r="37" spans="1:10">
       <c r="A37" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C37">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E37" s="4">
-        <v>63</v>
+        <v>3262</v>
       </c>
       <c r="F37" s="6">
-        <f t="shared" si="1"/>
-        <v>5.1391359888798887E-5</v>
+        <f>E37/$B$1</f>
+        <v>2.593734643930009E-3</v>
       </c>
       <c r="G37" s="4">
-        <v>89</v>
+        <v>5357</v>
       </c>
       <c r="H37" s="4"/>
       <c r="I37" s="4"/>
     </row>
+    <row r="38" spans="1:10">
+      <c r="A38" t="s">
+        <v>35</v>
+      </c>
+      <c r="B38" t="s">
+        <v>3</v>
+      </c>
+      <c r="C38">
+        <v>8</v>
+      </c>
+      <c r="E38" s="4">
+        <v>255</v>
+      </c>
+      <c r="F38" s="6">
+        <f>E38/$B$1</f>
+        <v>2.0275975910550345E-4</v>
+      </c>
+      <c r="G38" s="4">
+        <v>305</v>
+      </c>
+      <c r="H38" s="4"/>
+      <c r="I38" s="4"/>
+    </row>
+    <row r="41" spans="1:10">
+      <c r="J41" s="17"/>
+    </row>
+    <row r="42" spans="1:10">
+      <c r="A42" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="B42" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="C42" s="20">
+        <v>414</v>
+      </c>
+      <c r="D42" s="20">
+        <v>220</v>
+      </c>
+      <c r="E42" s="17">
+        <v>41066</v>
+      </c>
+      <c r="F42" s="19">
+        <v>0.03</v>
+      </c>
+      <c r="G42" s="20">
+        <v>92377</v>
+      </c>
+      <c r="H42" s="17"/>
+      <c r="I42" s="20">
+        <v>41066</v>
+      </c>
+      <c r="J42" s="17"/>
+    </row>
+    <row r="43" spans="1:10">
+      <c r="A43" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="B43" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="C43" s="20">
+        <v>3065</v>
+      </c>
+      <c r="D43" s="20">
+        <v>414</v>
+      </c>
+      <c r="E43" s="17">
+        <v>37283</v>
+      </c>
+      <c r="F43" s="19">
+        <v>0.03</v>
+      </c>
+      <c r="G43" s="20">
+        <v>84190</v>
+      </c>
+      <c r="H43" s="17"/>
+      <c r="I43" s="20">
+        <v>37283</v>
+      </c>
+      <c r="J43" s="17"/>
+    </row>
+    <row r="44" spans="1:10">
+      <c r="A44" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="B44" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="C44" s="18">
+        <v>220</v>
+      </c>
+      <c r="D44" s="18">
+        <v>7707728</v>
+      </c>
+      <c r="E44" s="16">
+        <v>281548</v>
+      </c>
+      <c r="F44" s="19">
+        <v>0.22</v>
+      </c>
+      <c r="G44" s="20">
+        <v>616429</v>
+      </c>
+      <c r="H44" s="20">
+        <f>I44-E42</f>
+        <v>240482</v>
+      </c>
+      <c r="I44" s="20">
+        <v>281548</v>
+      </c>
+    </row>
+    <row r="49" spans="5:5">
+      <c r="E49">
+        <v>372522</v>
+      </c>
+    </row>
+    <row r="58" spans="5:5" s="1" customFormat="1"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>